<commit_message>
under working,  receive all status under object chunk
</commit_message>
<xml_diff>
--- a/src/org/zaregoto/mqoparser/parser/tbl/states_tbl.xlsx
+++ b/src/org/zaregoto/mqoparser/parser/tbl/states_tbl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="states_tbl.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5620" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5620" uniqueCount="219">
   <si>
     <t>NOP</t>
   </si>
@@ -516,6 +516,246 @@
   </si>
   <si>
     <t>ReadObjectFaceCRS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Idle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectUid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFolding</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectScale</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectRotation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectTranslation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectPatch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectPatchtri</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectSegment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVisible</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectLocking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectShading</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFacet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectColorType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectColor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectMirror</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectMirrorAxis</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectMirrorDis</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectLathe</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectLatheAxis</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectLatheSeg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectBVertex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttrUid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttrColor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttrUid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttrWeit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttrColor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectVertexAttr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectBVertex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectBVertex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectBVertex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectBVertexVector</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectBVertexWeit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectBVertexColor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFaceV</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFaceM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFaceUV</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFaceCRS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFaceCOL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReadObjectFace</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -558,7 +798,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +815,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
@@ -794,7 +1040,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -811,6 +1057,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1150,8 +1401,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="BO53" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="BT71" sqref="BT71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1432,7 +1686,7 @@
         <v>83</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>76</v>
+        <v>159</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>76</v>
@@ -9549,236 +9803,236 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:77">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:77" s="17" customFormat="1">
+      <c r="A37" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="I37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J37" s="6" t="s">
+      <c r="J37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="K37" s="6" t="s">
+      <c r="K37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="L37" s="6" t="s">
+      <c r="L37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="M37" s="6" t="s">
+      <c r="M37" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="N37" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="O37" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="P37" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="N37" s="6" t="s">
+      <c r="R37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="O37" s="6" t="s">
+      <c r="S37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="P37" s="6" t="s">
+      <c r="T37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="Q37" s="6" t="s">
+      <c r="U37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="R37" s="6" t="s">
+      <c r="V37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="S37" s="6" t="s">
+      <c r="W37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="T37" s="6" t="s">
+      <c r="X37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="U37" s="6" t="s">
+      <c r="Y37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="V37" s="6" t="s">
+      <c r="Z37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="W37" s="6" t="s">
+      <c r="AA37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="X37" s="6" t="s">
+      <c r="AB37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="Y37" s="6" t="s">
+      <c r="AC37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="Z37" s="6" t="s">
+      <c r="AD37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AA37" s="6" t="s">
+      <c r="AE37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AB37" s="6" t="s">
+      <c r="AF37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AC37" s="6" t="s">
+      <c r="AG37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AD37" s="6" t="s">
+      <c r="AH37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AE37" s="6" t="s">
+      <c r="AI37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AF37" s="6" t="s">
+      <c r="AJ37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AG37" s="6" t="s">
+      <c r="AK37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AH37" s="6" t="s">
+      <c r="AL37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AI37" s="6" t="s">
+      <c r="AM37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AJ37" s="6" t="s">
+      <c r="AN37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AK37" s="6" t="s">
+      <c r="AO37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AL37" s="6" t="s">
+      <c r="AP37" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ37" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="AR37" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AS37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AM37" s="6" t="s">
+      <c r="AT37" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU37" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="AV37" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="AW37" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="AX37" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY37" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="AZ37" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="BA37" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="BB37" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="BC37" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="BD37" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="BE37" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="BF37" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="BG37" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="BH37" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="BI37" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ37" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="BK37" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="BL37" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AN37" s="6" t="s">
+      <c r="BN37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AO37" s="6" t="s">
+      <c r="BO37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AP37" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AQ37" s="6" t="s">
+      <c r="BP37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AR37" s="6" t="s">
+      <c r="BQ37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AS37" s="6" t="s">
+      <c r="BR37" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="BS37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AT37" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AU37" s="6" t="s">
+      <c r="BT37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AV37" s="6" t="s">
+      <c r="BU37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AW37" s="6" t="s">
+      <c r="BV37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AX37" s="6" t="s">
+      <c r="BW37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AY37" s="6" t="s">
+      <c r="BX37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="AZ37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BA37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BB37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BC37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BD37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BE37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BF37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BG37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BH37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BI37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BJ37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BK37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BL37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BM37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BN37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BO37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BP37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BQ37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BR37" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BS37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BT37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BU37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BV37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BW37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BX37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BY37" s="7" t="s">
+      <c r="BY37" s="19" t="s">
         <v>83</v>
       </c>
     </row>
@@ -10478,7 +10732,7 @@
         <v>115</v>
       </c>
       <c r="BY40" s="7" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:77">
@@ -10711,7 +10965,7 @@
         <v>116</v>
       </c>
       <c r="BY41" s="7" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:77">
@@ -10944,7 +11198,7 @@
         <v>118</v>
       </c>
       <c r="BY42" s="7" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:77">
@@ -11177,7 +11431,7 @@
         <v>119</v>
       </c>
       <c r="BY43" s="7" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:77">
@@ -11410,7 +11664,7 @@
         <v>120</v>
       </c>
       <c r="BY44" s="7" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:77">
@@ -11643,7 +11897,7 @@
         <v>121</v>
       </c>
       <c r="BY45" s="7" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:77">
@@ -11876,7 +12130,7 @@
         <v>122</v>
       </c>
       <c r="BY46" s="7" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:77">
@@ -12109,7 +12363,7 @@
         <v>123</v>
       </c>
       <c r="BY47" s="7" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:77">
@@ -12342,7 +12596,7 @@
         <v>124</v>
       </c>
       <c r="BY48" s="7" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:77">
@@ -12575,7 +12829,7 @@
         <v>125</v>
       </c>
       <c r="BY49" s="7" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:77">
@@ -12808,7 +13062,7 @@
         <v>126</v>
       </c>
       <c r="BY50" s="7" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:77">
@@ -13041,7 +13295,7 @@
         <v>127</v>
       </c>
       <c r="BY51" s="7" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:77">
@@ -13274,7 +13528,7 @@
         <v>128</v>
       </c>
       <c r="BY52" s="7" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:77">
@@ -13507,7 +13761,7 @@
         <v>129</v>
       </c>
       <c r="BY53" s="7" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:77">
@@ -13740,7 +13994,7 @@
         <v>130</v>
       </c>
       <c r="BY54" s="7" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:77">
@@ -13973,7 +14227,7 @@
         <v>131</v>
       </c>
       <c r="BY55" s="7" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:77">
@@ -14206,7 +14460,7 @@
         <v>132</v>
       </c>
       <c r="BY56" s="7" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:77">
@@ -14439,7 +14693,7 @@
         <v>133</v>
       </c>
       <c r="BY57" s="7" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:77">
@@ -14672,7 +14926,7 @@
         <v>134</v>
       </c>
       <c r="BY58" s="7" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:77">
@@ -14884,7 +15138,7 @@
         <v>135</v>
       </c>
       <c r="BR59" s="6" t="s">
-        <v>135</v>
+        <v>188</v>
       </c>
       <c r="BS59" s="6" t="s">
         <v>135</v>
@@ -14908,702 +15162,702 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:77">
+    <row r="60" spans="1:77" s="20" customFormat="1">
       <c r="A60" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="F60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="G60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="H60" s="6" t="s">
+      <c r="H60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="I60" s="6" t="s">
+      <c r="I60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="J60" s="6" t="s">
+      <c r="J60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="K60" s="6" t="s">
+      <c r="K60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="L60" s="6" t="s">
+      <c r="L60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="M60" s="6" t="s">
+      <c r="M60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="N60" s="6" t="s">
+      <c r="N60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="O60" s="6" t="s">
+      <c r="O60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="P60" s="6" t="s">
+      <c r="P60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="Q60" s="6" t="s">
+      <c r="Q60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="R60" s="6" t="s">
+      <c r="R60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="S60" s="6" t="s">
+      <c r="S60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="T60" s="6" t="s">
+      <c r="T60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="U60" s="6" t="s">
+      <c r="U60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="V60" s="6" t="s">
+      <c r="V60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="W60" s="6" t="s">
+      <c r="W60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="X60" s="6" t="s">
+      <c r="X60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="Y60" s="6" t="s">
+      <c r="Y60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="Z60" s="6" t="s">
+      <c r="Z60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AA60" s="6" t="s">
+      <c r="AA60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AB60" s="6" t="s">
+      <c r="AB60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AC60" s="6" t="s">
+      <c r="AC60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AD60" s="6" t="s">
+      <c r="AD60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AE60" s="6" t="s">
+      <c r="AE60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AF60" s="6" t="s">
+      <c r="AF60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AG60" s="6" t="s">
+      <c r="AG60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AH60" s="6" t="s">
+      <c r="AH60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AI60" s="6" t="s">
+      <c r="AI60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AJ60" s="6" t="s">
+      <c r="AJ60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AK60" s="6" t="s">
+      <c r="AK60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AL60" s="6" t="s">
+      <c r="AL60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AM60" s="6" t="s">
+      <c r="AM60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AN60" s="6" t="s">
+      <c r="AN60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AO60" s="6" t="s">
+      <c r="AO60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AP60" s="6" t="s">
+      <c r="AP60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AQ60" s="6" t="s">
+      <c r="AQ60" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="AR60" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="AS60" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="AT60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AR60" s="6" t="s">
+      <c r="AU60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AS60" s="6" t="s">
+      <c r="AV60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AT60" s="6" t="s">
+      <c r="AW60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AU60" s="6" t="s">
+      <c r="AX60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AV60" s="6" t="s">
+      <c r="AY60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AW60" s="6" t="s">
+      <c r="AZ60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AX60" s="6" t="s">
+      <c r="BA60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AY60" s="6" t="s">
+      <c r="BB60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AZ60" s="6" t="s">
+      <c r="BC60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BA60" s="6" t="s">
+      <c r="BD60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BB60" s="6" t="s">
+      <c r="BE60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BC60" s="6" t="s">
+      <c r="BF60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BD60" s="6" t="s">
+      <c r="BG60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BE60" s="6" t="s">
+      <c r="BH60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BF60" s="6" t="s">
+      <c r="BI60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BG60" s="6" t="s">
+      <c r="BJ60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BH60" s="6" t="s">
+      <c r="BK60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BI60" s="6" t="s">
+      <c r="BL60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BJ60" s="6" t="s">
+      <c r="BM60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BK60" s="6" t="s">
+      <c r="BN60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BL60" s="6" t="s">
+      <c r="BO60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BM60" s="6" t="s">
+      <c r="BP60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BN60" s="6" t="s">
+      <c r="BQ60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BO60" s="6" t="s">
+      <c r="BR60" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="BS60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BP60" s="6" t="s">
+      <c r="BT60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BQ60" s="6" t="s">
+      <c r="BU60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BR60" s="6" t="s">
+      <c r="BV60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BS60" s="6" t="s">
+      <c r="BW60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BT60" s="6" t="s">
+      <c r="BX60" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="BU60" s="6" t="s">
+      <c r="BY60" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="BV60" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="BW60" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="BX60" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="BY60" s="7" t="s">
-        <v>136</v>
-      </c>
     </row>
-    <row r="61" spans="1:77">
+    <row r="61" spans="1:77" s="20" customFormat="1">
       <c r="A61" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="F61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="G61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H61" s="6" t="s">
+      <c r="H61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="I61" s="6" t="s">
+      <c r="I61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="J61" s="6" t="s">
+      <c r="J61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="K61" s="6" t="s">
+      <c r="K61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="L61" s="6" t="s">
+      <c r="L61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="M61" s="6" t="s">
+      <c r="M61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="N61" s="6" t="s">
+      <c r="N61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="O61" s="6" t="s">
+      <c r="O61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="P61" s="6" t="s">
+      <c r="P61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="Q61" s="6" t="s">
+      <c r="Q61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="R61" s="6" t="s">
+      <c r="R61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="S61" s="6" t="s">
+      <c r="S61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="T61" s="6" t="s">
+      <c r="T61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="U61" s="6" t="s">
+      <c r="U61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="V61" s="6" t="s">
+      <c r="V61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="W61" s="6" t="s">
+      <c r="W61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="X61" s="6" t="s">
+      <c r="X61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="Y61" s="6" t="s">
+      <c r="Y61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="Z61" s="6" t="s">
+      <c r="Z61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AA61" s="6" t="s">
+      <c r="AA61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AB61" s="6" t="s">
+      <c r="AB61" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AC61" s="6" t="s">
+      <c r="AD61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AD61" s="6" t="s">
+      <c r="AE61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AE61" s="6" t="s">
+      <c r="AF61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AF61" s="6" t="s">
+      <c r="AG61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AG61" s="6" t="s">
+      <c r="AH61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AH61" s="6" t="s">
+      <c r="AI61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AI61" s="6" t="s">
+      <c r="AJ61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AJ61" s="6" t="s">
+      <c r="AK61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AK61" s="6" t="s">
+      <c r="AL61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AL61" s="6" t="s">
+      <c r="AM61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AM61" s="6" t="s">
+      <c r="AN61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AN61" s="6" t="s">
+      <c r="AO61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AO61" s="6" t="s">
+      <c r="AP61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AP61" s="6" t="s">
+      <c r="AQ61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AQ61" s="6" t="s">
+      <c r="AR61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AR61" s="6" t="s">
+      <c r="AS61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AS61" s="6" t="s">
+      <c r="AT61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AT61" s="6" t="s">
+      <c r="AU61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AU61" s="6" t="s">
+      <c r="AV61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AV61" s="6" t="s">
+      <c r="AW61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AW61" s="6" t="s">
+      <c r="AX61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AX61" s="6" t="s">
+      <c r="AY61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AY61" s="6" t="s">
+      <c r="AZ61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AZ61" s="6" t="s">
+      <c r="BA61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BA61" s="6" t="s">
+      <c r="BB61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BB61" s="6" t="s">
+      <c r="BC61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BC61" s="6" t="s">
+      <c r="BD61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BD61" s="6" t="s">
+      <c r="BE61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BE61" s="6" t="s">
+      <c r="BF61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BF61" s="6" t="s">
+      <c r="BG61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BG61" s="6" t="s">
+      <c r="BH61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BH61" s="6" t="s">
+      <c r="BI61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BI61" s="6" t="s">
+      <c r="BJ61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BJ61" s="6" t="s">
+      <c r="BK61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BK61" s="6" t="s">
+      <c r="BL61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BL61" s="6" t="s">
+      <c r="BM61" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="BN61" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="BO61" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="BP61" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="BQ61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BM61" s="6" t="s">
+      <c r="BR61" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="BS61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BN61" s="6" t="s">
+      <c r="BT61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BO61" s="6" t="s">
+      <c r="BU61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BP61" s="6" t="s">
+      <c r="BV61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BQ61" s="6" t="s">
+      <c r="BW61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BR61" s="6" t="s">
+      <c r="BX61" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="BS61" s="6" t="s">
+      <c r="BY61" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="BT61" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BU61" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BV61" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BW61" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BX61" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BY61" s="7" t="s">
-        <v>137</v>
-      </c>
     </row>
-    <row r="62" spans="1:77">
+    <row r="62" spans="1:77" s="20" customFormat="1">
       <c r="A62" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="F62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="G62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="H62" s="6" t="s">
+      <c r="H62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="I62" s="6" t="s">
+      <c r="I62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="J62" s="6" t="s">
+      <c r="J62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="K62" s="6" t="s">
+      <c r="K62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="L62" s="6" t="s">
+      <c r="L62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="M62" s="6" t="s">
+      <c r="M62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="N62" s="6" t="s">
+      <c r="N62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="O62" s="6" t="s">
+      <c r="O62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="P62" s="6" t="s">
+      <c r="P62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="Q62" s="6" t="s">
+      <c r="Q62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="R62" s="6" t="s">
+      <c r="R62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="S62" s="6" t="s">
+      <c r="S62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="T62" s="6" t="s">
+      <c r="T62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="U62" s="6" t="s">
+      <c r="U62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="V62" s="6" t="s">
+      <c r="V62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="W62" s="6" t="s">
+      <c r="W62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="X62" s="6" t="s">
+      <c r="X62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="Y62" s="6" t="s">
+      <c r="Y62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="Z62" s="6" t="s">
+      <c r="Z62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AA62" s="6" t="s">
+      <c r="AA62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AB62" s="6" t="s">
+      <c r="AB62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AC62" s="6" t="s">
+      <c r="AC62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AD62" s="6" t="s">
+      <c r="AD62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AE62" s="6" t="s">
+      <c r="AE62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AF62" s="6" t="s">
+      <c r="AF62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AG62" s="6" t="s">
+      <c r="AG62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AH62" s="6" t="s">
+      <c r="AH62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AI62" s="6" t="s">
+      <c r="AI62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AJ62" s="6" t="s">
+      <c r="AJ62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AK62" s="6" t="s">
+      <c r="AK62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AL62" s="6" t="s">
+      <c r="AL62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AM62" s="6" t="s">
+      <c r="AM62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AN62" s="6" t="s">
+      <c r="AN62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AO62" s="6" t="s">
+      <c r="AO62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AP62" s="6" t="s">
+      <c r="AP62" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="AQ62" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="AR62" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="AS62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AQ62" s="6" t="s">
+      <c r="AT62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AR62" s="6" t="s">
+      <c r="AU62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AS62" s="6" t="s">
+      <c r="AV62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AT62" s="6" t="s">
+      <c r="AW62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AU62" s="6" t="s">
+      <c r="AX62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AV62" s="6" t="s">
+      <c r="AY62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AW62" s="6" t="s">
+      <c r="AZ62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AX62" s="6" t="s">
+      <c r="BA62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AY62" s="6" t="s">
+      <c r="BB62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="AZ62" s="6" t="s">
+      <c r="BC62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BA62" s="6" t="s">
+      <c r="BD62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BB62" s="6" t="s">
+      <c r="BE62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BC62" s="6" t="s">
+      <c r="BF62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BD62" s="6" t="s">
+      <c r="BG62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BE62" s="6" t="s">
+      <c r="BH62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BF62" s="6" t="s">
+      <c r="BI62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BG62" s="6" t="s">
+      <c r="BJ62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BH62" s="6" t="s">
+      <c r="BK62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BI62" s="6" t="s">
+      <c r="BL62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BJ62" s="6" t="s">
+      <c r="BM62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BK62" s="6" t="s">
+      <c r="BN62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BL62" s="6" t="s">
+      <c r="BO62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BM62" s="6" t="s">
+      <c r="BP62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BN62" s="6" t="s">
+      <c r="BQ62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BO62" s="6" t="s">
+      <c r="BR62" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="BS62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BP62" s="6" t="s">
+      <c r="BT62" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="BU62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BQ62" s="6" t="s">
+      <c r="BV62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BR62" s="6" t="s">
+      <c r="BW62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BS62" s="6" t="s">
+      <c r="BX62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="BT62" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BU62" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BV62" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BW62" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BX62" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="BY62" s="7" t="s">
+      <c r="BY62" s="19" t="s">
         <v>151</v>
       </c>
     </row>
@@ -15816,13 +16070,13 @@
         <v>152</v>
       </c>
       <c r="BR63" s="6" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="BS63" s="6" t="s">
         <v>152</v>
       </c>
       <c r="BT63" s="6" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="BU63" s="6" t="s">
         <v>152</v>
@@ -16049,13 +16303,13 @@
         <v>141</v>
       </c>
       <c r="BR64" s="6" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="BS64" s="6" t="s">
         <v>141</v>
       </c>
       <c r="BT64" s="6" t="s">
-        <v>141</v>
+        <v>195</v>
       </c>
       <c r="BU64" s="6" t="s">
         <v>141</v>
@@ -16282,13 +16536,13 @@
         <v>142</v>
       </c>
       <c r="BR65" s="6" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="BS65" s="6" t="s">
         <v>142</v>
       </c>
       <c r="BT65" s="6" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="BU65" s="6" t="s">
         <v>142</v>
@@ -16515,7 +16769,7 @@
         <v>153</v>
       </c>
       <c r="BR66" s="6" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="BS66" s="6" t="s">
         <v>153</v>
@@ -16748,7 +17002,7 @@
         <v>154</v>
       </c>
       <c r="BR67" s="6" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
       <c r="BS67" s="6" t="s">
         <v>154</v>
@@ -16981,7 +17235,7 @@
         <v>155</v>
       </c>
       <c r="BR68" s="6" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="BS68" s="6" t="s">
         <v>155</v>
@@ -17214,13 +17468,13 @@
         <v>146</v>
       </c>
       <c r="BR69" s="6" t="s">
-        <v>146</v>
+        <v>201</v>
       </c>
       <c r="BS69" s="6" t="s">
         <v>146</v>
       </c>
       <c r="BT69" s="6" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="BU69" s="6" t="s">
         <v>146</v>
@@ -17447,13 +17701,13 @@
         <v>156</v>
       </c>
       <c r="BR70" s="6" t="s">
-        <v>156</v>
+        <v>202</v>
       </c>
       <c r="BS70" s="6" t="s">
         <v>156</v>
       </c>
       <c r="BT70" s="6" t="s">
-        <v>156</v>
+        <v>215</v>
       </c>
       <c r="BU70" s="6" t="s">
         <v>156</v>
@@ -17680,13 +17934,13 @@
         <v>148</v>
       </c>
       <c r="BR71" s="6" t="s">
-        <v>148</v>
+        <v>203</v>
       </c>
       <c r="BS71" s="6" t="s">
         <v>148</v>
       </c>
       <c r="BT71" s="6" t="s">
-        <v>148</v>
+        <v>216</v>
       </c>
       <c r="BU71" s="6" t="s">
         <v>148</v>
@@ -17913,13 +18167,13 @@
         <v>157</v>
       </c>
       <c r="BR72" s="6" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
       <c r="BS72" s="6" t="s">
         <v>157</v>
       </c>
       <c r="BT72" s="6" t="s">
-        <v>157</v>
+        <v>217</v>
       </c>
       <c r="BU72" s="6" t="s">
         <v>157</v>
@@ -18146,13 +18400,13 @@
         <v>158</v>
       </c>
       <c r="BR73" s="9" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="BS73" s="9" t="s">
         <v>158</v>
       </c>
       <c r="BT73" s="9" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="BU73" s="9" t="s">
         <v>158</v>

</xml_diff>